<commit_message>
tu vung bai 29
</commit_message>
<xml_diff>
--- a/tu-da-hoc.xlsx
+++ b/tu-da-hoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\japanese\kanji-game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EC132F-7528-41BD-931C-B7112BE91CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93E1F98-E119-4DA3-8BE5-F0A090EBAA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9B5C92A4-BC93-4E98-B3C8-5639172B51DA}"/>
+    <workbookView xWindow="7788" yWindow="0" windowWidth="15348" windowHeight="12336" xr2:uid="{9B5C92A4-BC93-4E98-B3C8-5639172B51DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="364">
   <si>
     <t>おくれます</t>
   </si>
@@ -924,6 +924,222 @@
   </si>
   <si>
     <t>chụp ảnh</t>
+  </si>
+  <si>
+    <t>こみます</t>
+  </si>
+  <si>
+    <t>すきます</t>
+  </si>
+  <si>
+    <t>こわれます</t>
+  </si>
+  <si>
+    <t>われます</t>
+  </si>
+  <si>
+    <t>おれます</t>
+  </si>
+  <si>
+    <t>やぶれます</t>
+  </si>
+  <si>
+    <t>よごれます</t>
+  </si>
+  <si>
+    <t>はずれます</t>
+  </si>
+  <si>
+    <t>とまります</t>
+  </si>
+  <si>
+    <t>まちがえます</t>
+  </si>
+  <si>
+    <t>かかります</t>
+  </si>
+  <si>
+    <t>おとします</t>
+  </si>
+  <si>
+    <t>さら</t>
+  </si>
+  <si>
+    <t>ちゃわん</t>
+  </si>
+  <si>
+    <t>コップ</t>
+  </si>
+  <si>
+    <t>クラス</t>
+  </si>
+  <si>
+    <t>ふくろ</t>
+  </si>
+  <si>
+    <t>さいふ</t>
+  </si>
+  <si>
+    <t>えだ</t>
+  </si>
+  <si>
+    <t>えきいん</t>
+  </si>
+  <si>
+    <t>このへん</t>
+  </si>
+  <si>
+    <t>へん</t>
+  </si>
+  <si>
+    <t>このぐらい</t>
+  </si>
+  <si>
+    <t>おさきにどうぞ</t>
+  </si>
+  <si>
+    <t>込みます</t>
+  </si>
+  <si>
+    <t>壊れます</t>
+  </si>
+  <si>
+    <t>割れます</t>
+  </si>
+  <si>
+    <t>折れます</t>
+  </si>
+  <si>
+    <t>破れます</t>
+  </si>
+  <si>
+    <t>汚れます</t>
+  </si>
+  <si>
+    <t>付きます</t>
+  </si>
+  <si>
+    <t>外れます</t>
+  </si>
+  <si>
+    <t>止まります</t>
+  </si>
+  <si>
+    <t>落とします</t>
+  </si>
+  <si>
+    <t>掛かります</t>
+  </si>
+  <si>
+    <t>「お」皿</t>
+  </si>
+  <si>
+    <t>袋</t>
+  </si>
+  <si>
+    <t>財布</t>
+  </si>
+  <si>
+    <t>枝</t>
+  </si>
+  <si>
+    <t>駅員</t>
+  </si>
+  <si>
+    <t>この辺</t>
+  </si>
+  <si>
+    <t>辺</t>
+  </si>
+  <si>
+    <t>お先にどうぞ</t>
+  </si>
+  <si>
+    <t>mở (cửa)</t>
+  </si>
+  <si>
+    <t>đóng (cửa)</t>
+  </si>
+  <si>
+    <t>sáng (điện)</t>
+  </si>
+  <si>
+    <t>tắt (điện)</t>
+  </si>
+  <si>
+    <t>đông, tắc (đường)</t>
+  </si>
+  <si>
+    <t>vắng, thoáng (đường)</t>
+  </si>
+  <si>
+    <t>hỏng (cái ghế bị)</t>
+  </si>
+  <si>
+    <t>vỡ (cái cốc bị)</t>
+  </si>
+  <si>
+    <t>gãy (cái cây bị)</t>
+  </si>
+  <si>
+    <t>rách (tờ giấy bị)</t>
+  </si>
+  <si>
+    <t>bắn (quần áo bị)</t>
+  </si>
+  <si>
+    <t>có, có gắn, có kèm theo (túi)</t>
+  </si>
+  <si>
+    <t>tuột, bung (cái cúc bị)</t>
+  </si>
+  <si>
+    <t>dừng (thang máy)</t>
+  </si>
+  <si>
+    <t>nhầm, sai</t>
+  </si>
+  <si>
+    <t>đánh rơi</t>
+  </si>
+  <si>
+    <t>khóa (chìa khóa)</t>
+  </si>
+  <si>
+    <t>cái đĩa</t>
+  </si>
+  <si>
+    <t>cái bát</t>
+  </si>
+  <si>
+    <t>cái cốc</t>
+  </si>
+  <si>
+    <t>thủy tinh</t>
+  </si>
+  <si>
+    <t>cái túi</t>
+  </si>
+  <si>
+    <t>cái ví</t>
+  </si>
+  <si>
+    <t>cành cây</t>
+  </si>
+  <si>
+    <t>nhân viên nhà ga</t>
+  </si>
+  <si>
+    <t>xung quanh đây, gần đây</t>
+  </si>
+  <si>
+    <t>xung quanh, chỗ</t>
+  </si>
+  <si>
+    <t>khoảng gần này</t>
+  </si>
+  <si>
+    <t>Xin mời đi trước</t>
   </si>
 </sst>
 </file>
@@ -1319,10 +1535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9766C5-377E-4030-93B0-E189C4D323FF}">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="69" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91:C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="57.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2724,7 +2940,393 @@
         <v>28</v>
       </c>
     </row>
+    <row r="91" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="H91" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="H92" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="H93" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="H94" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="H95" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="H96" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="H97" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="H98" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="H99" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="H100" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="H101" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="H102" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="H103" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="H104" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="H105" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="H106" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="H107" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="H108" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="H109" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="H110" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="H111" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="H112" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="H113" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="H114" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="H115" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="H116" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="H117" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="H118" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="H119" s="5">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>